<commit_message>
Agregado eventos y funcionalidad varios.
</commit_message>
<xml_diff>
--- a/Resolucion ej221.xlsx
+++ b/Resolucion ej221.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>Planteo</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>interrupción espera colectivo</t>
+  </si>
+  <si>
+    <t>Estado Parada</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -279,6 +282,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -744,10 +750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AB4"/>
+  <dimension ref="A2:AC4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,17 +767,17 @@
     <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="10" max="11" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C2" s="8" t="s">
         <v>33</v>
       </c>
@@ -786,22 +792,23 @@
         <v>36</v>
       </c>
       <c r="J2" s="9"/>
-      <c r="R2" s="8" t="s">
+      <c r="K2" s="10"/>
+      <c r="S2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="W2" s="8" t="s">
+      <c r="T2" s="8"/>
+      <c r="X2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AA2" s="8"/>
       <c r="AB2" s="8"/>
-    </row>
-    <row r="3" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+      <c r="AC2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -833,73 +840,76 @@
         <v>44</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="60" x14ac:dyDescent="0.25">
-      <c r="Y4" s="1" t="s">
+    <row r="4" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z4" s="1" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AA2:AC2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>